<commit_message>
Wijzigingen en aanvullingen lineaire regressie
</commit_message>
<xml_diff>
--- a/_book/data/economiedata.xlsx
+++ b/_book/data/economiedata.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\office\statistiek-excel\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\studieboeken\excelanalyse\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F97DF687-A7D2-4196-A678-74538BC30A70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F657E8C7-270D-4AD1-8A9F-8D139574D06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED2FDF92-1070-47F9-A1BB-D38CB9F58A41}"/>
   </bookViews>
   <sheets>
-    <sheet name="economiedata" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -116,305 +113,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="C1"/>
-      <sheetName val="C2"/>
-      <sheetName val="N1"/>
-      <sheetName val="CN"/>
-      <sheetName val="N2"/>
-      <sheetName val="Blad1"/>
-      <sheetName val="sim1"/>
-      <sheetName val="sim2"/>
-      <sheetName val="economiedata"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8">
-        <row r="1">
-          <cell r="E1" t="str">
-            <v>Aandelenindex</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="C2">
-            <v>1.75</v>
-          </cell>
-          <cell r="D2">
-            <v>6.1</v>
-          </cell>
-          <cell r="E2">
-            <v>719</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="C3">
-            <v>1.75</v>
-          </cell>
-          <cell r="D3">
-            <v>6.2</v>
-          </cell>
-          <cell r="E3">
-            <v>704</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="C4">
-            <v>1.75</v>
-          </cell>
-          <cell r="D4">
-            <v>6.2</v>
-          </cell>
-          <cell r="E4">
-            <v>822</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="C5">
-            <v>1.75</v>
-          </cell>
-          <cell r="D5">
-            <v>5.9</v>
-          </cell>
-          <cell r="E5">
-            <v>876</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6">
-            <v>1.75</v>
-          </cell>
-          <cell r="D6">
-            <v>6.1</v>
-          </cell>
-          <cell r="E6">
-            <v>866</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>1.75</v>
-          </cell>
-          <cell r="D7">
-            <v>6.1</v>
-          </cell>
-          <cell r="E7">
-            <v>884</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>1.75</v>
-          </cell>
-          <cell r="D8">
-            <v>6.1</v>
-          </cell>
-          <cell r="E8">
-            <v>949</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9">
-            <v>1.75</v>
-          </cell>
-          <cell r="D9">
-            <v>6.2</v>
-          </cell>
-          <cell r="E9">
-            <v>971</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10">
-            <v>1.75</v>
-          </cell>
-          <cell r="D10">
-            <v>6.1</v>
-          </cell>
-          <cell r="E10">
-            <v>958</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>1.75</v>
-          </cell>
-          <cell r="D11">
-            <v>5.8</v>
-          </cell>
-          <cell r="E11">
-            <v>943</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>1.75</v>
-          </cell>
-          <cell r="D12">
-            <v>5.9</v>
-          </cell>
-          <cell r="E12">
-            <v>965</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>2</v>
-          </cell>
-          <cell r="D13">
-            <v>6</v>
-          </cell>
-          <cell r="E13">
-            <v>1047</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>2</v>
-          </cell>
-          <cell r="D14">
-            <v>5.9</v>
-          </cell>
-          <cell r="E14">
-            <v>1075</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>2</v>
-          </cell>
-          <cell r="D15">
-            <v>5.7</v>
-          </cell>
-          <cell r="E15">
-            <v>1130</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16">
-            <v>2.25</v>
-          </cell>
-          <cell r="D16">
-            <v>5.6</v>
-          </cell>
-          <cell r="E16">
-            <v>1167</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17">
-            <v>2.25</v>
-          </cell>
-          <cell r="D17">
-            <v>5.5</v>
-          </cell>
-          <cell r="E17">
-            <v>1159</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18">
-            <v>2.25</v>
-          </cell>
-          <cell r="D18">
-            <v>5.5</v>
-          </cell>
-          <cell r="E18">
-            <v>1195</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19">
-            <v>2.5</v>
-          </cell>
-          <cell r="D19">
-            <v>5.5</v>
-          </cell>
-          <cell r="E19">
-            <v>1234</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20">
-            <v>2.5</v>
-          </cell>
-          <cell r="D20">
-            <v>5.6</v>
-          </cell>
-          <cell r="E20">
-            <v>1254</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21">
-            <v>2.5</v>
-          </cell>
-          <cell r="D21">
-            <v>5.4</v>
-          </cell>
-          <cell r="E21">
-            <v>1256</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22">
-            <v>2.5</v>
-          </cell>
-          <cell r="D22">
-            <v>5.3</v>
-          </cell>
-          <cell r="E22">
-            <v>1293</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23">
-            <v>2.5</v>
-          </cell>
-          <cell r="D23">
-            <v>5.3</v>
-          </cell>
-          <cell r="E23">
-            <v>1357</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>2.5</v>
-          </cell>
-          <cell r="D24">
-            <v>5.3</v>
-          </cell>
-          <cell r="E24">
-            <v>1394</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>2.75</v>
-          </cell>
-          <cell r="D25">
-            <v>5.3</v>
-          </cell>
-          <cell r="E25">
-            <v>1464</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -731,7 +429,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>